<commit_message>
Added getTarget to user rather than game.
</commit_message>
<xml_diff>
--- a/server/REST operations.xlsx
+++ b/server/REST operations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7170" windowHeight="7470" tabRatio="510" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7170" windowHeight="7470" tabRatio="510" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="POST" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
   <si>
     <t>/</t>
   </si>
@@ -152,15 +152,6 @@
     <t>{result:{duration:4, hugLimit:10, running:1, indoor:0, violence:0}}</t>
   </si>
   <si>
-    <t>/game/target</t>
-  </si>
-  <si>
-    <t>/game/hugs</t>
-  </si>
-  <si>
-    <t>gameID=1234, userID=2345</t>
-  </si>
-  <si>
     <t>/login</t>
   </si>
   <si>
@@ -173,9 +164,6 @@
     <t>{result:1234}</t>
   </si>
   <si>
-    <t>{result:23}</t>
-  </si>
-  <si>
     <t>{result:2.23}</t>
   </si>
   <si>
@@ -231,6 +219,9 @@
   </si>
   <si>
     <t>/user/hugs/current</t>
+  </si>
+  <si>
+    <t>/user/target</t>
   </si>
 </sst>
 </file>
@@ -622,10 +613,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +680,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
@@ -700,7 +691,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
@@ -711,76 +702,76 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
@@ -789,80 +780,69 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>48</v>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
         <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" t="s">
         <v>38</v>
       </c>
     </row>
@@ -878,7 +858,7 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -905,10 +885,10 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -924,23 +904,23 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -951,7 +931,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -962,13 +942,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -976,10 +956,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -987,10 +967,10 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -998,10 +978,10 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1034,18 +1014,18 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>